<commit_message>
year 1996 to 2012
</commit_message>
<xml_diff>
--- a/Data/Ballard Locks Fish Counts/Ballardcohocounts2012.xlsx
+++ b/Data/Ballard Locks Fish Counts/Ballardcohocounts2012.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elizabeth Allyn\Documents\GitHub\PinnipedCaseStudies\Data\Ballard Locks Fish Counts\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92629EBC-00E4-41C8-88ED-A042E88C9287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="11370" windowHeight="7350"/>
+    <workbookView xWindow="1815" yWindow="1125" windowWidth="24960" windowHeight="14355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,18 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$N$38</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -75,13 +92,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0;[Red]&quot;-&quot;#,##0"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,7 +198,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -190,7 +207,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -232,44 +248,25 @@
     <xf numFmtId="1" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -289,13 +286,21 @@
       <color rgb="FFFFC000"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -333,7 +338,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -367,6 +372,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -401,9 +407,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -576,23 +583,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="N36" sqref="N36:N37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="7" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" customWidth="1"/>
@@ -1487,1822 +1494,1822 @@
     <col min="16144" max="16144" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="36" customFormat="1" ht="28.5">
-      <c r="D1" s="37"/>
-      <c r="E1" s="38" t="s">
+    <row r="1" spans="1:16" s="28" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D1" s="29"/>
+      <c r="E1" s="30" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="30" customHeight="1">
+    <row r="3" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="32" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="32"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="33" t="s">
+      <c r="E3" s="24"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="33"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="33" t="s">
+      <c r="I3" s="25"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:16" ht="30" customHeight="1">
+    <row r="4" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:16" s="4" customFormat="1" ht="24" customHeight="1">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="18" t="s">
+      <c r="J5" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="22" t="s">
+      <c r="K5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="22" t="s">
+      <c r="L5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="22" t="s">
+      <c r="M5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N5" s="22" t="s">
+      <c r="N5" s="7" t="s">
         <v>15</v>
       </c>
       <c r="O5" s="2"/>
       <c r="P5" s="3"/>
     </row>
-    <row r="6" spans="1:16" ht="24" customHeight="1">
-      <c r="A6" s="9">
-        <v>35309</v>
-      </c>
-      <c r="B6" s="22">
+    <row r="6" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
+        <v>41153</v>
+      </c>
+      <c r="B6" s="7">
         <v>3</v>
       </c>
-      <c r="C6" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="14">
+      <c r="C6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="13">
         <v>13</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="15">
         <v>8</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="17">
         <v>26</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="7">
         <v>5</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="14">
         <f t="shared" ref="H6:H8" si="0">SUM((D6/B6)*G6)</f>
         <v>21.666666666666664</v>
       </c>
-      <c r="I6" s="17">
+      <c r="I6" s="16">
         <f t="shared" ref="I6:J8" si="1">SUM((E6/110)*720)</f>
         <v>52.36363636363636</v>
       </c>
-      <c r="J6" s="19">
+      <c r="J6" s="18">
         <f t="shared" si="1"/>
         <v>170.18181818181819</v>
       </c>
-      <c r="K6" s="28">
+      <c r="K6" s="9">
         <f t="shared" ref="K6:K8" si="2">SUM(H6+I6+J6)</f>
         <v>244.21212121212122</v>
       </c>
-      <c r="L6" s="29">
+      <c r="L6" s="10">
         <f t="shared" ref="L6:L8" si="3">SUM(J6/(I6+J6))*100</f>
         <v>76.470588235294116</v>
       </c>
-      <c r="M6" s="29">
+      <c r="M6" s="10">
         <f>SUM(100-L6)</f>
         <v>23.529411764705884</v>
       </c>
-      <c r="N6" s="30">
+      <c r="N6" s="22">
         <v>244</v>
       </c>
-      <c r="O6" s="5"/>
-      <c r="P6" s="6"/>
-    </row>
-    <row r="7" spans="1:16" ht="24" customHeight="1">
-      <c r="A7" s="9">
-        <v>35310</v>
-      </c>
-      <c r="B7" s="22">
+      <c r="O6" s="4"/>
+      <c r="P6" s="5"/>
+    </row>
+    <row r="7" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
+        <v>41154</v>
+      </c>
+      <c r="B7" s="7">
         <v>4</v>
       </c>
-      <c r="C7" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="14">
+      <c r="C7" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="13">
         <v>1</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="15">
         <v>11</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="17">
         <v>30</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="7">
         <v>6</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="14">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="I7" s="17">
+      <c r="I7" s="16">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
-      <c r="J7" s="19">
+      <c r="J7" s="18">
         <f t="shared" si="1"/>
         <v>196.36363636363635</v>
       </c>
-      <c r="K7" s="28">
+      <c r="K7" s="9">
         <f t="shared" si="2"/>
         <v>269.86363636363637</v>
       </c>
-      <c r="L7" s="29">
+      <c r="L7" s="10">
         <f t="shared" si="3"/>
         <v>73.17073170731706</v>
       </c>
-      <c r="M7" s="29">
+      <c r="M7" s="10">
         <f t="shared" ref="M7:M11" si="4">SUM(100-L7)</f>
         <v>26.82926829268294</v>
       </c>
-      <c r="N7" s="31">
+      <c r="N7" s="23">
         <f>SUM(N6,K7)</f>
         <v>513.86363636363637</v>
       </c>
       <c r="O7" s="2"/>
-      <c r="P7" s="6"/>
-    </row>
-    <row r="8" spans="1:16" ht="24" customHeight="1">
-      <c r="A8" s="9">
-        <v>35311</v>
-      </c>
-      <c r="B8" s="22">
+      <c r="P7" s="5"/>
+    </row>
+    <row r="8" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8">
+        <v>41155</v>
+      </c>
+      <c r="B8" s="7">
         <v>5</v>
       </c>
-      <c r="C8" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="14">
-        <v>0</v>
-      </c>
-      <c r="E8" s="16">
+      <c r="C8" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="13">
+        <v>0</v>
+      </c>
+      <c r="E8" s="15">
         <v>18</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="17">
         <v>57</v>
       </c>
-      <c r="G8" s="22">
+      <c r="G8" s="7">
         <v>7</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I8" s="17">
+      <c r="I8" s="16">
         <f t="shared" si="1"/>
         <v>117.81818181818181</v>
       </c>
-      <c r="J8" s="19">
+      <c r="J8" s="18">
         <f t="shared" si="1"/>
         <v>373.09090909090912</v>
       </c>
-      <c r="K8" s="28">
+      <c r="K8" s="9">
         <f t="shared" si="2"/>
         <v>490.90909090909093</v>
       </c>
-      <c r="L8" s="29">
+      <c r="L8" s="10">
         <f t="shared" si="3"/>
         <v>76</v>
       </c>
-      <c r="M8" s="29">
+      <c r="M8" s="10">
         <f t="shared" si="4"/>
         <v>24</v>
       </c>
-      <c r="N8" s="31">
+      <c r="N8" s="23">
         <f>SUM(N7,K8)</f>
         <v>1004.7727272727273</v>
       </c>
       <c r="O8" s="2"/>
-      <c r="P8" s="6"/>
-    </row>
-    <row r="9" spans="1:16" ht="24" customHeight="1">
-      <c r="A9" s="9">
-        <v>35312</v>
-      </c>
-      <c r="B9" s="23">
+      <c r="P8" s="5"/>
+    </row>
+    <row r="9" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
+        <v>41156</v>
+      </c>
+      <c r="B9" s="7">
         <v>5</v>
       </c>
-      <c r="C9" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="20">
+      <c r="C9" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="13">
         <v>103</v>
       </c>
-      <c r="E9" s="26">
+      <c r="E9" s="15">
         <v>5</v>
       </c>
-      <c r="F9" s="27">
+      <c r="F9" s="21">
         <v>37</v>
       </c>
-      <c r="G9" s="25">
+      <c r="G9" s="20">
         <v>5</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="14">
         <f t="shared" ref="H9:H37" si="5">SUM((D9/B9)*G9)</f>
         <v>103</v>
       </c>
-      <c r="I9" s="17">
+      <c r="I9" s="16">
         <f t="shared" ref="I9:J37" si="6">SUM((E9/110)*720)</f>
         <v>32.727272727272727</v>
       </c>
-      <c r="J9" s="19">
+      <c r="J9" s="18">
         <f t="shared" si="6"/>
         <v>242.18181818181819</v>
       </c>
-      <c r="K9" s="28">
+      <c r="K9" s="9">
         <f t="shared" ref="K9:K11" si="7">SUM(H9+I9+J9)</f>
         <v>377.90909090909088</v>
       </c>
-      <c r="L9" s="29">
+      <c r="L9" s="10">
         <f t="shared" ref="L9:L11" si="8">SUM(J9/(I9+J9))*100</f>
         <v>88.095238095238088</v>
       </c>
-      <c r="M9" s="29">
+      <c r="M9" s="10">
         <f t="shared" si="4"/>
         <v>11.904761904761912</v>
       </c>
-      <c r="N9" s="31">
+      <c r="N9" s="23">
         <f>SUM(N8,K9)</f>
         <v>1382.681818181818</v>
       </c>
-      <c r="O9" s="5"/>
-      <c r="P9" s="6"/>
-    </row>
-    <row r="10" spans="1:16" ht="24" customHeight="1">
-      <c r="A10" s="9">
-        <v>35313</v>
-      </c>
-      <c r="B10" s="22">
+      <c r="O9" s="4"/>
+      <c r="P9" s="5"/>
+    </row>
+    <row r="10" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="8">
+        <v>41157</v>
+      </c>
+      <c r="B10" s="7">
         <v>4</v>
       </c>
-      <c r="C10" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="14">
-        <v>0</v>
-      </c>
-      <c r="E10" s="16">
+      <c r="C10" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="13">
+        <v>0</v>
+      </c>
+      <c r="E10" s="15">
         <v>25</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="17">
         <v>76</v>
       </c>
-      <c r="G10" s="22">
+      <c r="G10" s="7">
         <v>12</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="14">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I10" s="17">
+      <c r="I10" s="16">
         <f t="shared" si="6"/>
         <v>163.63636363636363</v>
       </c>
-      <c r="J10" s="19">
+      <c r="J10" s="18">
         <f t="shared" si="6"/>
         <v>497.45454545454544</v>
       </c>
-      <c r="K10" s="28">
+      <c r="K10" s="9">
         <f t="shared" si="7"/>
         <v>661.09090909090901</v>
       </c>
-      <c r="L10" s="29">
+      <c r="L10" s="10">
         <f t="shared" si="8"/>
         <v>75.247524752475258</v>
       </c>
-      <c r="M10" s="29">
+      <c r="M10" s="10">
         <f t="shared" si="4"/>
         <v>24.752475247524742</v>
       </c>
-      <c r="N10" s="31">
+      <c r="N10" s="23">
         <f>SUM(N9,K10)</f>
         <v>2043.772727272727</v>
       </c>
       <c r="O10" s="2"/>
-      <c r="P10" s="6"/>
-    </row>
-    <row r="11" spans="1:16" ht="24" customHeight="1">
-      <c r="A11" s="9">
-        <v>35314</v>
-      </c>
-      <c r="B11" s="22">
+      <c r="P10" s="5"/>
+    </row>
+    <row r="11" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
+        <v>41158</v>
+      </c>
+      <c r="B11" s="7">
         <v>2</v>
       </c>
-      <c r="C11" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="14">
+      <c r="C11" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="15">
         <v>13</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="17">
         <v>51</v>
       </c>
-      <c r="G11" s="22">
+      <c r="G11" s="7">
         <v>4</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="14">
         <f t="shared" si="5"/>
         <v>20</v>
       </c>
-      <c r="I11" s="17">
+      <c r="I11" s="16">
         <f t="shared" si="6"/>
         <v>85.090909090909093</v>
       </c>
-      <c r="J11" s="19">
+      <c r="J11" s="18">
         <f t="shared" si="6"/>
         <v>333.81818181818181</v>
       </c>
-      <c r="K11" s="28">
+      <c r="K11" s="9">
         <f t="shared" si="7"/>
         <v>438.90909090909088</v>
       </c>
-      <c r="L11" s="29">
+      <c r="L11" s="10">
         <f t="shared" si="8"/>
         <v>79.6875</v>
       </c>
-      <c r="M11" s="29">
+      <c r="M11" s="10">
         <f t="shared" si="4"/>
         <v>20.3125</v>
       </c>
-      <c r="N11" s="31">
+      <c r="N11" s="23">
         <f>SUM(N10,K11)</f>
         <v>2482.681818181818</v>
       </c>
       <c r="O11" s="2"/>
-      <c r="P11" s="6"/>
-    </row>
-    <row r="12" spans="1:16" ht="24" customHeight="1">
-      <c r="A12" s="9">
-        <v>35315</v>
-      </c>
-      <c r="B12" s="22">
+      <c r="P11" s="5"/>
+    </row>
+    <row r="12" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="8">
+        <v>41159</v>
+      </c>
+      <c r="B12" s="7">
         <v>3</v>
       </c>
-      <c r="C12" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" s="14">
+      <c r="C12" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="13">
         <v>19</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E12" s="15">
         <v>23</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="17">
         <v>68</v>
       </c>
-      <c r="G12" s="22">
+      <c r="G12" s="7">
         <v>9</v>
       </c>
-      <c r="H12" s="15">
+      <c r="H12" s="14">
         <f t="shared" si="5"/>
         <v>57</v>
       </c>
-      <c r="I12" s="17">
+      <c r="I12" s="16">
         <f t="shared" si="6"/>
         <v>150.54545454545453</v>
       </c>
-      <c r="J12" s="19">
+      <c r="J12" s="18">
         <f t="shared" si="6"/>
         <v>445.09090909090907</v>
       </c>
-      <c r="K12" s="28">
+      <c r="K12" s="9">
         <f t="shared" ref="K12:K37" si="9">SUM(H12+I12+J12)</f>
         <v>652.63636363636363</v>
       </c>
-      <c r="L12" s="29">
+      <c r="L12" s="10">
         <f t="shared" ref="L12:L37" si="10">SUM(J12/(I12+J12))*100</f>
         <v>74.72527472527473</v>
       </c>
-      <c r="M12" s="29">
+      <c r="M12" s="10">
         <f t="shared" ref="M12:M14" si="11">SUM(100-L12)</f>
         <v>25.27472527472527</v>
       </c>
-      <c r="N12" s="31">
+      <c r="N12" s="23">
         <f t="shared" ref="N12:N14" si="12">SUM(N11,K12)</f>
         <v>3135.3181818181815</v>
       </c>
       <c r="O12" s="2"/>
-      <c r="P12" s="6"/>
-    </row>
-    <row r="13" spans="1:16" ht="24" customHeight="1">
-      <c r="A13" s="9">
-        <v>35316</v>
-      </c>
-      <c r="B13" s="22">
+      <c r="P12" s="5"/>
+    </row>
+    <row r="13" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="8">
+        <v>41160</v>
+      </c>
+      <c r="B13" s="7">
         <v>4</v>
       </c>
-      <c r="C13" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D13" s="14">
-        <v>0</v>
-      </c>
-      <c r="E13" s="16">
+      <c r="C13" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="13">
+        <v>0</v>
+      </c>
+      <c r="E13" s="15">
         <v>26</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="17">
         <v>112</v>
       </c>
-      <c r="G13" s="22">
+      <c r="G13" s="7">
         <v>9</v>
       </c>
-      <c r="H13" s="15">
+      <c r="H13" s="14">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I13" s="17">
+      <c r="I13" s="16">
         <f t="shared" si="6"/>
         <v>170.18181818181819</v>
       </c>
-      <c r="J13" s="19">
+      <c r="J13" s="18">
         <f t="shared" si="6"/>
         <v>733.09090909090901</v>
       </c>
-      <c r="K13" s="28">
+      <c r="K13" s="9">
         <f t="shared" si="9"/>
         <v>903.27272727272725</v>
       </c>
-      <c r="L13" s="29">
+      <c r="L13" s="10">
         <f t="shared" si="10"/>
         <v>81.159420289855063</v>
       </c>
-      <c r="M13" s="29">
+      <c r="M13" s="10">
         <f t="shared" si="11"/>
         <v>18.840579710144937</v>
       </c>
-      <c r="N13" s="31">
+      <c r="N13" s="23">
         <f t="shared" si="12"/>
         <v>4038.590909090909</v>
       </c>
-      <c r="O13" s="5"/>
-      <c r="P13" s="6"/>
-    </row>
-    <row r="14" spans="1:16" ht="24" customHeight="1">
-      <c r="A14" s="9">
-        <v>35317</v>
-      </c>
-      <c r="B14" s="22">
+      <c r="O13" s="4"/>
+      <c r="P13" s="5"/>
+    </row>
+    <row r="14" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="8">
+        <v>41161</v>
+      </c>
+      <c r="B14" s="7">
         <v>6</v>
       </c>
-      <c r="C14" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14" s="14">
+      <c r="C14" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="13">
         <v>118</v>
       </c>
-      <c r="E14" s="16">
+      <c r="E14" s="15">
         <v>57</v>
       </c>
-      <c r="F14" s="18">
+      <c r="F14" s="17">
         <v>173</v>
       </c>
-      <c r="G14" s="22">
+      <c r="G14" s="7">
         <v>8</v>
       </c>
-      <c r="H14" s="15">
+      <c r="H14" s="14">
         <f t="shared" si="5"/>
         <v>157.33333333333334</v>
       </c>
-      <c r="I14" s="17">
+      <c r="I14" s="16">
         <f t="shared" si="6"/>
         <v>373.09090909090912</v>
       </c>
-      <c r="J14" s="19">
+      <c r="J14" s="18">
         <f t="shared" si="6"/>
         <v>1132.3636363636365</v>
       </c>
-      <c r="K14" s="28">
+      <c r="K14" s="9">
         <f t="shared" si="9"/>
         <v>1662.787878787879</v>
       </c>
-      <c r="L14" s="29">
+      <c r="L14" s="10">
         <f t="shared" si="10"/>
         <v>75.217391304347842</v>
       </c>
-      <c r="M14" s="29">
+      <c r="M14" s="10">
         <f t="shared" si="11"/>
         <v>24.782608695652158</v>
       </c>
-      <c r="N14" s="31">
+      <c r="N14" s="23">
         <f t="shared" si="12"/>
         <v>5701.378787878788</v>
       </c>
       <c r="O14" s="2"/>
-      <c r="P14" s="6"/>
-    </row>
-    <row r="15" spans="1:16" ht="24" customHeight="1">
-      <c r="A15" s="9">
-        <v>35318</v>
-      </c>
-      <c r="B15" s="22">
+      <c r="P14" s="5"/>
+    </row>
+    <row r="15" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="8">
+        <v>41162</v>
+      </c>
+      <c r="B15" s="7">
         <v>4</v>
       </c>
-      <c r="C15" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D15" s="14">
+      <c r="C15" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="13">
         <v>38</v>
       </c>
-      <c r="E15" s="16">
+      <c r="E15" s="15">
         <v>55</v>
       </c>
-      <c r="F15" s="18">
+      <c r="F15" s="17">
         <v>143</v>
       </c>
-      <c r="G15" s="22">
+      <c r="G15" s="7">
         <v>9</v>
       </c>
-      <c r="H15" s="15">
+      <c r="H15" s="14">
         <f t="shared" si="5"/>
         <v>85.5</v>
       </c>
-      <c r="I15" s="17">
+      <c r="I15" s="16">
         <f t="shared" si="6"/>
         <v>360</v>
       </c>
-      <c r="J15" s="19">
+      <c r="J15" s="18">
         <f t="shared" si="6"/>
         <v>936</v>
       </c>
-      <c r="K15" s="28">
+      <c r="K15" s="9">
         <f t="shared" si="9"/>
         <v>1381.5</v>
       </c>
-      <c r="L15" s="29">
+      <c r="L15" s="10">
         <f t="shared" si="10"/>
         <v>72.222222222222214</v>
       </c>
-      <c r="M15" s="29">
+      <c r="M15" s="10">
         <f t="shared" ref="M15:M16" si="13">SUM(100-L15)</f>
         <v>27.777777777777786</v>
       </c>
-      <c r="N15" s="31">
+      <c r="N15" s="23">
         <f t="shared" ref="N15:N16" si="14">SUM(N14,K15)</f>
         <v>7082.878787878788</v>
       </c>
       <c r="O15" s="2"/>
-      <c r="P15" s="6"/>
-    </row>
-    <row r="16" spans="1:16" ht="24" customHeight="1">
-      <c r="A16" s="9">
-        <v>35319</v>
-      </c>
-      <c r="B16" s="22">
+      <c r="P15" s="5"/>
+    </row>
+    <row r="16" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="8">
+        <v>41163</v>
+      </c>
+      <c r="B16" s="7">
         <v>5</v>
       </c>
-      <c r="C16" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" s="14">
+      <c r="C16" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="13">
         <v>333</v>
       </c>
-      <c r="E16" s="16">
+      <c r="E16" s="15">
         <v>63</v>
       </c>
-      <c r="F16" s="18">
+      <c r="F16" s="17">
         <v>177</v>
       </c>
-      <c r="G16" s="22">
+      <c r="G16" s="7">
         <v>8</v>
       </c>
-      <c r="H16" s="15">
+      <c r="H16" s="14">
         <f t="shared" si="5"/>
         <v>532.79999999999995</v>
       </c>
-      <c r="I16" s="17">
+      <c r="I16" s="16">
         <f t="shared" si="6"/>
         <v>412.36363636363637</v>
       </c>
-      <c r="J16" s="19">
+      <c r="J16" s="18">
         <f t="shared" si="6"/>
         <v>1158.5454545454545</v>
       </c>
-      <c r="K16" s="28">
+      <c r="K16" s="9">
         <f t="shared" si="9"/>
         <v>2103.7090909090907</v>
       </c>
-      <c r="L16" s="29">
+      <c r="L16" s="10">
         <f t="shared" si="10"/>
         <v>73.75</v>
       </c>
-      <c r="M16" s="29">
+      <c r="M16" s="10">
         <f t="shared" si="13"/>
         <v>26.25</v>
       </c>
-      <c r="N16" s="31">
+      <c r="N16" s="23">
         <f t="shared" si="14"/>
         <v>9186.5878787878792</v>
       </c>
       <c r="O16" s="2"/>
-      <c r="P16" s="6"/>
-    </row>
-    <row r="17" spans="1:16" ht="24" customHeight="1">
-      <c r="A17" s="9">
-        <v>35320</v>
-      </c>
-      <c r="B17" s="22">
+      <c r="P16" s="5"/>
+    </row>
+    <row r="17" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="8">
+        <v>41164</v>
+      </c>
+      <c r="B17" s="7">
         <v>3</v>
       </c>
-      <c r="C17" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D17" s="14">
+      <c r="C17" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="13">
         <v>152</v>
       </c>
-      <c r="E17" s="16">
+      <c r="E17" s="15">
         <v>36</v>
       </c>
-      <c r="F17" s="18">
+      <c r="F17" s="17">
         <v>136</v>
       </c>
-      <c r="G17" s="22">
+      <c r="G17" s="7">
         <v>7</v>
       </c>
-      <c r="H17" s="15">
+      <c r="H17" s="14">
         <f t="shared" si="5"/>
         <v>354.66666666666663</v>
       </c>
-      <c r="I17" s="17">
+      <c r="I17" s="16">
         <f t="shared" si="6"/>
         <v>235.63636363636363</v>
       </c>
-      <c r="J17" s="19">
+      <c r="J17" s="18">
         <f t="shared" si="6"/>
         <v>890.18181818181813</v>
       </c>
-      <c r="K17" s="28">
+      <c r="K17" s="9">
         <f t="shared" si="9"/>
         <v>1480.4848484848485</v>
       </c>
-      <c r="L17" s="29">
+      <c r="L17" s="10">
         <f t="shared" si="10"/>
         <v>79.069767441860463</v>
       </c>
-      <c r="M17" s="29">
+      <c r="M17" s="10">
         <f t="shared" ref="M17:M37" si="15">SUM(100-L17)</f>
         <v>20.930232558139537</v>
       </c>
-      <c r="N17" s="31">
+      <c r="N17" s="23">
         <f t="shared" ref="N17:N37" si="16">SUM(N16,K17)</f>
         <v>10667.072727272727</v>
       </c>
       <c r="O17" s="2"/>
-      <c r="P17" s="6"/>
-    </row>
-    <row r="18" spans="1:16" ht="24" customHeight="1">
-      <c r="A18" s="9">
-        <v>35321</v>
-      </c>
-      <c r="B18" s="22">
+      <c r="P17" s="5"/>
+    </row>
+    <row r="18" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="8">
+        <v>41165</v>
+      </c>
+      <c r="B18" s="7">
         <v>7</v>
       </c>
-      <c r="C18" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D18" s="14">
+      <c r="C18" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="13">
         <v>51</v>
       </c>
-      <c r="E18" s="16">
+      <c r="E18" s="15">
         <v>52</v>
       </c>
-      <c r="F18" s="18">
+      <c r="F18" s="17">
         <v>161</v>
       </c>
-      <c r="G18" s="22">
+      <c r="G18" s="7">
         <v>13</v>
       </c>
-      <c r="H18" s="15">
+      <c r="H18" s="14">
         <f t="shared" si="5"/>
         <v>94.714285714285708</v>
       </c>
-      <c r="I18" s="17">
+      <c r="I18" s="16">
         <f t="shared" si="6"/>
         <v>340.36363636363637</v>
       </c>
-      <c r="J18" s="19">
+      <c r="J18" s="18">
         <f t="shared" si="6"/>
         <v>1053.8181818181818</v>
       </c>
-      <c r="K18" s="28">
+      <c r="K18" s="9">
         <f t="shared" si="9"/>
         <v>1488.8961038961038</v>
       </c>
-      <c r="L18" s="29">
+      <c r="L18" s="10">
         <f t="shared" si="10"/>
         <v>75.586854460093903</v>
       </c>
-      <c r="M18" s="29">
+      <c r="M18" s="10">
         <f t="shared" si="15"/>
         <v>24.413145539906097</v>
       </c>
-      <c r="N18" s="31">
+      <c r="N18" s="23">
         <f t="shared" si="16"/>
         <v>12155.968831168831</v>
       </c>
       <c r="O18" s="2"/>
-      <c r="P18" s="6"/>
-    </row>
-    <row r="19" spans="1:16" ht="24" customHeight="1">
-      <c r="A19" s="9">
-        <v>35322</v>
-      </c>
-      <c r="B19" s="22">
+      <c r="P18" s="5"/>
+    </row>
+    <row r="19" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="8">
+        <v>41166</v>
+      </c>
+      <c r="B19" s="7">
         <v>4</v>
       </c>
-      <c r="C19" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="14">
+      <c r="C19" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="13">
         <v>130</v>
       </c>
-      <c r="E19" s="16">
+      <c r="E19" s="15">
         <v>28</v>
       </c>
-      <c r="F19" s="18">
+      <c r="F19" s="17">
         <v>87</v>
       </c>
-      <c r="G19" s="22">
+      <c r="G19" s="7">
         <v>6</v>
       </c>
-      <c r="H19" s="15">
+      <c r="H19" s="14">
         <f t="shared" si="5"/>
         <v>195</v>
       </c>
-      <c r="I19" s="17">
+      <c r="I19" s="16">
         <f t="shared" si="6"/>
         <v>183.27272727272725</v>
       </c>
-      <c r="J19" s="19">
+      <c r="J19" s="18">
         <f t="shared" si="6"/>
         <v>569.4545454545455</v>
       </c>
-      <c r="K19" s="28">
+      <c r="K19" s="9">
         <f t="shared" si="9"/>
         <v>947.72727272727275</v>
       </c>
-      <c r="L19" s="29">
+      <c r="L19" s="10">
         <f t="shared" si="10"/>
         <v>75.652173913043484</v>
       </c>
-      <c r="M19" s="29">
+      <c r="M19" s="10">
         <f t="shared" si="15"/>
         <v>24.347826086956516</v>
       </c>
-      <c r="N19" s="31">
+      <c r="N19" s="23">
         <f t="shared" si="16"/>
         <v>13103.696103896104</v>
       </c>
       <c r="O19" s="2"/>
-      <c r="P19" s="6"/>
-    </row>
-    <row r="20" spans="1:16" ht="24" customHeight="1">
-      <c r="A20" s="9">
-        <v>35323</v>
-      </c>
-      <c r="B20" s="22">
+      <c r="P19" s="5"/>
+    </row>
+    <row r="20" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="8">
+        <v>41167</v>
+      </c>
+      <c r="B20" s="7">
         <v>4</v>
       </c>
-      <c r="C20" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D20" s="14">
+      <c r="C20" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="13">
         <v>135</v>
       </c>
-      <c r="E20" s="16">
+      <c r="E20" s="15">
         <v>79</v>
       </c>
-      <c r="F20" s="18">
+      <c r="F20" s="17">
         <v>181</v>
       </c>
-      <c r="G20" s="22">
+      <c r="G20" s="7">
         <v>5</v>
       </c>
-      <c r="H20" s="15">
+      <c r="H20" s="14">
         <f t="shared" si="5"/>
         <v>168.75</v>
       </c>
-      <c r="I20" s="17">
+      <c r="I20" s="16">
         <f t="shared" si="6"/>
         <v>517.09090909090901</v>
       </c>
-      <c r="J20" s="19">
+      <c r="J20" s="18">
         <f t="shared" si="6"/>
         <v>1184.7272727272727</v>
       </c>
-      <c r="K20" s="28">
+      <c r="K20" s="9">
         <f t="shared" si="9"/>
         <v>1870.5681818181818</v>
       </c>
-      <c r="L20" s="29">
+      <c r="L20" s="10">
         <f t="shared" si="10"/>
         <v>69.615384615384627</v>
       </c>
-      <c r="M20" s="29">
+      <c r="M20" s="10">
         <f t="shared" si="15"/>
         <v>30.384615384615373</v>
       </c>
-      <c r="N20" s="31">
+      <c r="N20" s="23">
         <f t="shared" si="16"/>
         <v>14974.264285714286</v>
       </c>
       <c r="O20" s="2"/>
-      <c r="P20" s="6"/>
-    </row>
-    <row r="21" spans="1:16" ht="24" customHeight="1">
-      <c r="A21" s="9">
-        <v>35324</v>
-      </c>
-      <c r="B21" s="22">
+      <c r="P20" s="5"/>
+    </row>
+    <row r="21" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="8">
+        <v>41168</v>
+      </c>
+      <c r="B21" s="7">
         <v>3</v>
       </c>
-      <c r="C21" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D21" s="14">
+      <c r="C21" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="13">
         <v>305</v>
       </c>
-      <c r="E21" s="16">
+      <c r="E21" s="15">
         <v>47</v>
       </c>
-      <c r="F21" s="18">
+      <c r="F21" s="17">
         <v>141</v>
       </c>
-      <c r="G21" s="22">
+      <c r="G21" s="7">
         <v>8</v>
       </c>
-      <c r="H21" s="15">
+      <c r="H21" s="14">
         <f t="shared" si="5"/>
         <v>813.33333333333337</v>
       </c>
-      <c r="I21" s="17">
+      <c r="I21" s="16">
         <f t="shared" si="6"/>
         <v>307.63636363636363</v>
       </c>
-      <c r="J21" s="19">
+      <c r="J21" s="18">
         <f t="shared" si="6"/>
         <v>922.90909090909088</v>
       </c>
-      <c r="K21" s="28">
+      <c r="K21" s="9">
         <f t="shared" si="9"/>
         <v>2043.878787878788</v>
       </c>
-      <c r="L21" s="29">
+      <c r="L21" s="10">
         <f t="shared" si="10"/>
         <v>75</v>
       </c>
-      <c r="M21" s="29">
+      <c r="M21" s="10">
         <f t="shared" si="15"/>
         <v>25</v>
       </c>
-      <c r="N21" s="31">
+      <c r="N21" s="23">
         <f t="shared" si="16"/>
         <v>17018.143073593073</v>
       </c>
       <c r="O21" s="2"/>
-      <c r="P21" s="6"/>
-    </row>
-    <row r="22" spans="1:16" ht="24" customHeight="1">
-      <c r="A22" s="9">
-        <v>35325</v>
-      </c>
-      <c r="B22" s="22">
+      <c r="P21" s="5"/>
+    </row>
+    <row r="22" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="8">
+        <v>41169</v>
+      </c>
+      <c r="B22" s="7">
         <v>3</v>
       </c>
-      <c r="C22" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D22" s="14">
+      <c r="C22" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="13">
         <v>140</v>
       </c>
-      <c r="E22" s="16">
+      <c r="E22" s="15">
         <v>14</v>
       </c>
-      <c r="F22" s="18">
+      <c r="F22" s="17">
         <v>51</v>
       </c>
-      <c r="G22" s="22">
+      <c r="G22" s="7">
         <v>7</v>
       </c>
-      <c r="H22" s="15">
+      <c r="H22" s="14">
         <f t="shared" si="5"/>
         <v>326.66666666666663</v>
       </c>
-      <c r="I22" s="17">
+      <c r="I22" s="16">
         <f t="shared" si="6"/>
         <v>91.636363636363626</v>
       </c>
-      <c r="J22" s="19">
+      <c r="J22" s="18">
         <f t="shared" si="6"/>
         <v>333.81818181818181</v>
       </c>
-      <c r="K22" s="28">
+      <c r="K22" s="9">
         <f t="shared" si="9"/>
         <v>752.12121212121201</v>
       </c>
-      <c r="L22" s="29">
+      <c r="L22" s="10">
         <f t="shared" si="10"/>
         <v>78.461538461538467</v>
       </c>
-      <c r="M22" s="29">
+      <c r="M22" s="10">
         <f t="shared" si="15"/>
         <v>21.538461538461533</v>
       </c>
-      <c r="N22" s="31">
+      <c r="N22" s="23">
         <f t="shared" si="16"/>
         <v>17770.264285714286</v>
       </c>
       <c r="O22" s="2"/>
-      <c r="P22" s="6"/>
-    </row>
-    <row r="23" spans="1:16" ht="24" customHeight="1">
-      <c r="A23" s="9">
-        <v>35326</v>
-      </c>
-      <c r="B23" s="22">
+      <c r="P22" s="5"/>
+    </row>
+    <row r="23" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="8">
+        <v>41170</v>
+      </c>
+      <c r="B23" s="7">
         <v>4</v>
       </c>
-      <c r="C23" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D23" s="14">
+      <c r="C23" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="13">
         <v>42</v>
       </c>
-      <c r="E23" s="16">
+      <c r="E23" s="15">
         <v>25</v>
       </c>
-      <c r="F23" s="18">
+      <c r="F23" s="17">
         <v>69</v>
       </c>
-      <c r="G23" s="22">
+      <c r="G23" s="7">
         <v>10</v>
       </c>
-      <c r="H23" s="15">
+      <c r="H23" s="14">
         <f t="shared" si="5"/>
         <v>105</v>
       </c>
-      <c r="I23" s="17">
+      <c r="I23" s="16">
         <f t="shared" si="6"/>
         <v>163.63636363636363</v>
       </c>
-      <c r="J23" s="19">
+      <c r="J23" s="18">
         <f t="shared" si="6"/>
         <v>451.63636363636368</v>
       </c>
-      <c r="K23" s="28">
+      <c r="K23" s="9">
         <f t="shared" si="9"/>
         <v>720.27272727272725</v>
       </c>
-      <c r="L23" s="29">
+      <c r="L23" s="10">
         <f t="shared" si="10"/>
         <v>73.404255319148945</v>
       </c>
-      <c r="M23" s="29">
+      <c r="M23" s="10">
         <f t="shared" si="15"/>
         <v>26.595744680851055</v>
       </c>
-      <c r="N23" s="31">
+      <c r="N23" s="23">
         <f t="shared" si="16"/>
         <v>18490.537012987013</v>
       </c>
       <c r="O23" s="2"/>
-      <c r="P23" s="6"/>
-    </row>
-    <row r="24" spans="1:16" ht="24" customHeight="1">
-      <c r="A24" s="9">
-        <v>35327</v>
-      </c>
-      <c r="B24" s="22">
+      <c r="P23" s="5"/>
+    </row>
+    <row r="24" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="8">
+        <v>41171</v>
+      </c>
+      <c r="B24" s="7">
         <v>3</v>
       </c>
-      <c r="C24" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D24" s="14">
+      <c r="C24" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="13">
         <v>81</v>
       </c>
-      <c r="E24" s="16">
+      <c r="E24" s="15">
         <v>10</v>
       </c>
-      <c r="F24" s="18">
+      <c r="F24" s="17">
         <v>41</v>
       </c>
-      <c r="G24" s="22">
+      <c r="G24" s="7">
         <v>3</v>
       </c>
-      <c r="H24" s="15">
+      <c r="H24" s="14">
         <f t="shared" si="5"/>
         <v>81</v>
       </c>
-      <c r="I24" s="17">
+      <c r="I24" s="16">
         <f t="shared" si="6"/>
         <v>65.454545454545453</v>
       </c>
-      <c r="J24" s="19">
+      <c r="J24" s="18">
         <f t="shared" si="6"/>
         <v>268.36363636363637</v>
       </c>
-      <c r="K24" s="28">
+      <c r="K24" s="9">
         <f t="shared" si="9"/>
         <v>414.81818181818181</v>
       </c>
-      <c r="L24" s="29">
+      <c r="L24" s="10">
         <f t="shared" si="10"/>
         <v>80.392156862745097</v>
       </c>
-      <c r="M24" s="29">
+      <c r="M24" s="10">
         <f t="shared" si="15"/>
         <v>19.607843137254903</v>
       </c>
-      <c r="N24" s="31">
+      <c r="N24" s="23">
         <f t="shared" si="16"/>
         <v>18905.355194805194</v>
       </c>
       <c r="O24" s="2"/>
-      <c r="P24" s="6"/>
-    </row>
-    <row r="25" spans="1:16" ht="24" customHeight="1">
-      <c r="A25" s="9">
-        <v>35328</v>
-      </c>
-      <c r="B25" s="22">
+      <c r="P24" s="5"/>
+    </row>
+    <row r="25" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="8">
+        <v>41172</v>
+      </c>
+      <c r="B25" s="7">
         <v>1</v>
       </c>
-      <c r="C25" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D25" s="14">
-        <v>0</v>
-      </c>
-      <c r="E25" s="16">
+      <c r="C25" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="13">
+        <v>0</v>
+      </c>
+      <c r="E25" s="15">
         <v>23</v>
       </c>
-      <c r="F25" s="18">
+      <c r="F25" s="17">
         <v>72</v>
       </c>
-      <c r="G25" s="22">
+      <c r="G25" s="7">
         <v>1</v>
       </c>
-      <c r="H25" s="15">
+      <c r="H25" s="14">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I25" s="17">
+      <c r="I25" s="16">
         <f t="shared" si="6"/>
         <v>150.54545454545453</v>
       </c>
-      <c r="J25" s="19">
+      <c r="J25" s="18">
         <f t="shared" si="6"/>
         <v>471.27272727272725</v>
       </c>
-      <c r="K25" s="28">
+      <c r="K25" s="9">
         <f t="shared" si="9"/>
         <v>621.81818181818176</v>
       </c>
-      <c r="L25" s="29">
+      <c r="L25" s="10">
         <f t="shared" si="10"/>
         <v>75.789473684210535</v>
       </c>
-      <c r="M25" s="29">
+      <c r="M25" s="10">
         <f t="shared" si="15"/>
         <v>24.210526315789465</v>
       </c>
-      <c r="N25" s="31">
+      <c r="N25" s="23">
         <f t="shared" si="16"/>
         <v>19527.173376623374</v>
       </c>
       <c r="O25" s="2"/>
-      <c r="P25" s="6"/>
-    </row>
-    <row r="26" spans="1:16" ht="24" customHeight="1">
-      <c r="A26" s="9">
-        <v>35329</v>
-      </c>
-      <c r="B26" s="22">
+      <c r="P25" s="5"/>
+    </row>
+    <row r="26" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="8">
+        <v>41173</v>
+      </c>
+      <c r="B26" s="7">
         <v>4</v>
       </c>
-      <c r="C26" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D26" s="14">
+      <c r="C26" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="13">
         <v>20</v>
       </c>
-      <c r="E26" s="16">
+      <c r="E26" s="15">
         <v>11</v>
       </c>
-      <c r="F26" s="18">
+      <c r="F26" s="17">
         <v>38</v>
       </c>
-      <c r="G26" s="22">
+      <c r="G26" s="7">
         <v>8</v>
       </c>
-      <c r="H26" s="15">
+      <c r="H26" s="14">
         <f t="shared" si="5"/>
         <v>40</v>
       </c>
-      <c r="I26" s="17">
+      <c r="I26" s="16">
         <f t="shared" si="6"/>
         <v>72</v>
       </c>
-      <c r="J26" s="19">
+      <c r="J26" s="18">
         <f t="shared" si="6"/>
         <v>248.72727272727272</v>
       </c>
-      <c r="K26" s="28">
+      <c r="K26" s="9">
         <f t="shared" si="9"/>
         <v>360.72727272727275</v>
       </c>
-      <c r="L26" s="29">
+      <c r="L26" s="10">
         <f t="shared" si="10"/>
         <v>77.551020408163268</v>
       </c>
-      <c r="M26" s="29">
+      <c r="M26" s="10">
         <f t="shared" si="15"/>
         <v>22.448979591836732</v>
       </c>
-      <c r="N26" s="31">
+      <c r="N26" s="23">
         <f t="shared" si="16"/>
         <v>19887.900649350646</v>
       </c>
       <c r="O26" s="2"/>
-      <c r="P26" s="6"/>
-    </row>
-    <row r="27" spans="1:16" ht="24" customHeight="1">
-      <c r="A27" s="9">
-        <v>35330</v>
-      </c>
-      <c r="B27" s="22">
+      <c r="P26" s="5"/>
+    </row>
+    <row r="27" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="8">
+        <v>41174</v>
+      </c>
+      <c r="B27" s="7">
         <v>5</v>
       </c>
-      <c r="C27" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D27" s="14">
+      <c r="C27" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="13">
         <v>26</v>
       </c>
-      <c r="E27" s="16">
+      <c r="E27" s="15">
         <v>15</v>
       </c>
-      <c r="F27" s="18">
+      <c r="F27" s="17">
         <v>48</v>
       </c>
-      <c r="G27" s="22">
+      <c r="G27" s="7">
         <v>9</v>
       </c>
-      <c r="H27" s="15">
+      <c r="H27" s="14">
         <f t="shared" si="5"/>
         <v>46.800000000000004</v>
       </c>
-      <c r="I27" s="17">
+      <c r="I27" s="16">
         <f t="shared" si="6"/>
         <v>98.181818181818173</v>
       </c>
-      <c r="J27" s="19">
+      <c r="J27" s="18">
         <f t="shared" si="6"/>
         <v>314.18181818181819</v>
       </c>
-      <c r="K27" s="28">
+      <c r="K27" s="9">
         <f t="shared" si="9"/>
         <v>459.16363636363633</v>
       </c>
-      <c r="L27" s="29">
+      <c r="L27" s="10">
         <f t="shared" si="10"/>
         <v>76.19047619047619</v>
       </c>
-      <c r="M27" s="29">
+      <c r="M27" s="10">
         <f t="shared" si="15"/>
         <v>23.80952380952381</v>
       </c>
-      <c r="N27" s="31">
+      <c r="N27" s="23">
         <f t="shared" si="16"/>
         <v>20347.064285714281</v>
       </c>
       <c r="O27" s="2"/>
-      <c r="P27" s="6"/>
-    </row>
-    <row r="28" spans="1:16" ht="24" customHeight="1">
-      <c r="A28" s="9">
-        <v>35331</v>
-      </c>
-      <c r="B28" s="22">
+      <c r="P27" s="5"/>
+    </row>
+    <row r="28" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="8">
+        <v>41175</v>
+      </c>
+      <c r="B28" s="7">
         <v>6</v>
       </c>
-      <c r="C28" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D28" s="14">
+      <c r="C28" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="13">
         <v>74</v>
       </c>
-      <c r="E28" s="16">
+      <c r="E28" s="15">
         <v>33</v>
       </c>
-      <c r="F28" s="18">
+      <c r="F28" s="17">
         <v>93</v>
       </c>
-      <c r="G28" s="22">
+      <c r="G28" s="7">
         <v>10</v>
       </c>
-      <c r="H28" s="15">
+      <c r="H28" s="14">
         <f t="shared" si="5"/>
         <v>123.33333333333334</v>
       </c>
-      <c r="I28" s="17">
+      <c r="I28" s="16">
         <f t="shared" si="6"/>
         <v>216</v>
       </c>
-      <c r="J28" s="19">
+      <c r="J28" s="18">
         <f t="shared" si="6"/>
         <v>608.72727272727275</v>
       </c>
-      <c r="K28" s="28">
+      <c r="K28" s="9">
         <f t="shared" si="9"/>
         <v>948.06060606060612</v>
       </c>
-      <c r="L28" s="29">
+      <c r="L28" s="10">
         <f t="shared" si="10"/>
         <v>73.80952380952381</v>
       </c>
-      <c r="M28" s="29">
+      <c r="M28" s="10">
         <f t="shared" si="15"/>
         <v>26.19047619047619</v>
       </c>
-      <c r="N28" s="31">
+      <c r="N28" s="23">
         <f t="shared" si="16"/>
         <v>21295.124891774889</v>
       </c>
       <c r="O28" s="2"/>
-      <c r="P28" s="6"/>
-    </row>
-    <row r="29" spans="1:16" ht="24" customHeight="1">
-      <c r="A29" s="9">
-        <v>35332</v>
-      </c>
-      <c r="B29" s="22">
+      <c r="P28" s="5"/>
+    </row>
+    <row r="29" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="8">
+        <v>41176</v>
+      </c>
+      <c r="B29" s="7">
         <v>4</v>
       </c>
-      <c r="C29" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D29" s="14">
+      <c r="C29" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="13">
         <v>175</v>
       </c>
-      <c r="E29" s="16">
+      <c r="E29" s="15">
         <v>30</v>
       </c>
-      <c r="F29" s="18">
+      <c r="F29" s="17">
         <v>94</v>
       </c>
-      <c r="G29" s="22">
+      <c r="G29" s="7">
         <v>7</v>
       </c>
-      <c r="H29" s="15">
+      <c r="H29" s="14">
         <f t="shared" si="5"/>
         <v>306.25</v>
       </c>
-      <c r="I29" s="17">
+      <c r="I29" s="16">
         <f t="shared" si="6"/>
         <v>196.36363636363635</v>
       </c>
-      <c r="J29" s="19">
+      <c r="J29" s="18">
         <f t="shared" si="6"/>
         <v>615.27272727272725</v>
       </c>
-      <c r="K29" s="28">
+      <c r="K29" s="9">
         <f t="shared" si="9"/>
         <v>1117.8863636363635</v>
       </c>
-      <c r="L29" s="29">
+      <c r="L29" s="10">
         <f t="shared" si="10"/>
         <v>75.806451612903231</v>
       </c>
-      <c r="M29" s="29">
+      <c r="M29" s="10">
         <f t="shared" si="15"/>
         <v>24.193548387096769</v>
       </c>
-      <c r="N29" s="31">
+      <c r="N29" s="23">
         <f t="shared" si="16"/>
         <v>22413.011255411253</v>
       </c>
       <c r="O29" s="2"/>
-      <c r="P29" s="6"/>
-    </row>
-    <row r="30" spans="1:16" ht="24" customHeight="1">
-      <c r="A30" s="9">
-        <v>35333</v>
-      </c>
-      <c r="B30" s="22">
+      <c r="P29" s="5"/>
+    </row>
+    <row r="30" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="8">
+        <v>41177</v>
+      </c>
+      <c r="B30" s="7">
         <v>4</v>
       </c>
-      <c r="C30" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D30" s="14">
+      <c r="C30" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" s="13">
         <v>67</v>
       </c>
-      <c r="E30" s="16">
+      <c r="E30" s="15">
         <v>17</v>
       </c>
-      <c r="F30" s="18">
+      <c r="F30" s="17">
         <v>65</v>
       </c>
-      <c r="G30" s="22">
+      <c r="G30" s="7">
         <v>10</v>
       </c>
-      <c r="H30" s="15">
+      <c r="H30" s="14">
         <f t="shared" si="5"/>
         <v>167.5</v>
       </c>
-      <c r="I30" s="17">
+      <c r="I30" s="16">
         <f t="shared" si="6"/>
         <v>111.27272727272727</v>
       </c>
-      <c r="J30" s="19">
+      <c r="J30" s="18">
         <f t="shared" si="6"/>
         <v>425.4545454545455</v>
       </c>
-      <c r="K30" s="28">
+      <c r="K30" s="9">
         <f t="shared" si="9"/>
         <v>704.22727272727275</v>
       </c>
-      <c r="L30" s="29">
+      <c r="L30" s="10">
         <f t="shared" si="10"/>
         <v>79.268292682926827</v>
       </c>
-      <c r="M30" s="29">
+      <c r="M30" s="10">
         <f t="shared" si="15"/>
         <v>20.731707317073173</v>
       </c>
-      <c r="N30" s="31">
+      <c r="N30" s="23">
         <f t="shared" si="16"/>
         <v>23117.238528138525</v>
       </c>
       <c r="O30" s="2"/>
-      <c r="P30" s="6"/>
-    </row>
-    <row r="31" spans="1:16" ht="24" customHeight="1">
-      <c r="A31" s="9">
-        <v>35334</v>
-      </c>
-      <c r="B31" s="22">
+      <c r="P30" s="5"/>
+    </row>
+    <row r="31" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="8">
+        <v>41178</v>
+      </c>
+      <c r="B31" s="7">
         <v>4</v>
       </c>
-      <c r="C31" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D31" s="14">
+      <c r="C31" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" s="13">
         <v>244</v>
       </c>
-      <c r="E31" s="16">
+      <c r="E31" s="15">
         <v>23</v>
       </c>
-      <c r="F31" s="18">
+      <c r="F31" s="17">
         <v>92</v>
       </c>
-      <c r="G31" s="22">
+      <c r="G31" s="7">
         <v>8</v>
       </c>
-      <c r="H31" s="15">
+      <c r="H31" s="14">
         <f t="shared" si="5"/>
         <v>488</v>
       </c>
-      <c r="I31" s="17">
+      <c r="I31" s="16">
         <f t="shared" si="6"/>
         <v>150.54545454545453</v>
       </c>
-      <c r="J31" s="19">
+      <c r="J31" s="18">
         <f t="shared" si="6"/>
         <v>602.18181818181813</v>
       </c>
-      <c r="K31" s="28">
+      <c r="K31" s="9">
         <f t="shared" si="9"/>
         <v>1240.7272727272725</v>
       </c>
-      <c r="L31" s="29">
+      <c r="L31" s="10">
         <f t="shared" si="10"/>
         <v>80</v>
       </c>
-      <c r="M31" s="29">
+      <c r="M31" s="10">
         <f t="shared" si="15"/>
         <v>20</v>
       </c>
-      <c r="N31" s="31">
+      <c r="N31" s="23">
         <f t="shared" si="16"/>
         <v>24357.965800865797</v>
       </c>
       <c r="O31" s="2"/>
-      <c r="P31" s="6"/>
-    </row>
-    <row r="32" spans="1:16" ht="24" customHeight="1">
-      <c r="A32" s="9">
-        <v>35335</v>
-      </c>
-      <c r="B32" s="22">
+      <c r="P31" s="5"/>
+    </row>
+    <row r="32" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="8">
+        <v>41179</v>
+      </c>
+      <c r="B32" s="7">
         <v>3</v>
       </c>
-      <c r="C32" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D32" s="14">
+      <c r="C32" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" s="13">
         <v>606</v>
       </c>
-      <c r="E32" s="16">
+      <c r="E32" s="15">
         <v>19</v>
       </c>
-      <c r="F32" s="18">
+      <c r="F32" s="17">
         <v>53</v>
       </c>
-      <c r="G32" s="22">
+      <c r="G32" s="7">
         <v>4</v>
       </c>
-      <c r="H32" s="15">
+      <c r="H32" s="14">
         <f t="shared" si="5"/>
         <v>808</v>
       </c>
-      <c r="I32" s="17">
+      <c r="I32" s="16">
         <f t="shared" si="6"/>
         <v>124.36363636363636</v>
       </c>
-      <c r="J32" s="19">
+      <c r="J32" s="18">
         <f t="shared" si="6"/>
         <v>346.90909090909088</v>
       </c>
-      <c r="K32" s="28">
+      <c r="K32" s="9">
         <f t="shared" si="9"/>
         <v>1279.2727272727273</v>
       </c>
-      <c r="L32" s="29">
+      <c r="L32" s="10">
         <f t="shared" si="10"/>
         <v>73.6111111111111</v>
       </c>
-      <c r="M32" s="29">
+      <c r="M32" s="10">
         <f t="shared" si="15"/>
         <v>26.3888888888889</v>
       </c>
-      <c r="N32" s="31">
+      <c r="N32" s="23">
         <f t="shared" si="16"/>
         <v>25637.238528138525</v>
       </c>
       <c r="O32" s="2"/>
-      <c r="P32" s="6"/>
-    </row>
-    <row r="33" spans="1:16" ht="24" customHeight="1">
-      <c r="A33" s="9">
-        <v>35336</v>
-      </c>
-      <c r="B33" s="22">
+      <c r="P32" s="5"/>
+    </row>
+    <row r="33" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="8">
+        <v>41180</v>
+      </c>
+      <c r="B33" s="7">
         <v>3</v>
       </c>
-      <c r="C33" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D33" s="14">
+      <c r="C33" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" s="13">
         <v>115</v>
       </c>
-      <c r="E33" s="16">
+      <c r="E33" s="15">
         <v>29</v>
       </c>
-      <c r="F33" s="18">
+      <c r="F33" s="17">
         <v>69</v>
       </c>
-      <c r="G33" s="22">
+      <c r="G33" s="7">
         <v>5</v>
       </c>
-      <c r="H33" s="15">
+      <c r="H33" s="14">
         <f t="shared" si="5"/>
         <v>191.66666666666669</v>
       </c>
-      <c r="I33" s="17">
+      <c r="I33" s="16">
         <f t="shared" si="6"/>
         <v>189.81818181818181</v>
       </c>
-      <c r="J33" s="19">
+      <c r="J33" s="18">
         <f t="shared" si="6"/>
         <v>451.63636363636368</v>
       </c>
-      <c r="K33" s="28">
+      <c r="K33" s="9">
         <f t="shared" si="9"/>
         <v>833.12121212121224</v>
       </c>
-      <c r="L33" s="29">
+      <c r="L33" s="10">
         <f t="shared" si="10"/>
         <v>70.408163265306129</v>
       </c>
-      <c r="M33" s="29">
+      <c r="M33" s="10">
         <f t="shared" si="15"/>
         <v>29.591836734693871</v>
       </c>
-      <c r="N33" s="31">
+      <c r="N33" s="23">
         <f t="shared" si="16"/>
         <v>26470.359740259737</v>
       </c>
       <c r="O33" s="2"/>
-      <c r="P33" s="6"/>
-    </row>
-    <row r="34" spans="1:16" ht="24" customHeight="1">
-      <c r="A34" s="9">
-        <v>35337</v>
-      </c>
-      <c r="B34" s="22">
+      <c r="P33" s="5"/>
+    </row>
+    <row r="34" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="8">
+        <v>41181</v>
+      </c>
+      <c r="B34" s="7">
         <v>3</v>
       </c>
-      <c r="C34" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D34" s="14">
+      <c r="C34" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" s="13">
         <v>15</v>
       </c>
-      <c r="E34" s="16">
+      <c r="E34" s="15">
         <v>15</v>
       </c>
-      <c r="F34" s="18">
+      <c r="F34" s="17">
         <v>39</v>
       </c>
-      <c r="G34" s="22">
+      <c r="G34" s="7">
         <v>4</v>
       </c>
-      <c r="H34" s="15">
+      <c r="H34" s="14">
         <f t="shared" si="5"/>
         <v>20</v>
       </c>
-      <c r="I34" s="17">
+      <c r="I34" s="16">
         <f t="shared" si="6"/>
         <v>98.181818181818173</v>
       </c>
-      <c r="J34" s="19">
+      <c r="J34" s="18">
         <f t="shared" si="6"/>
         <v>255.27272727272728</v>
       </c>
-      <c r="K34" s="28">
+      <c r="K34" s="9">
         <f t="shared" si="9"/>
         <v>373.45454545454544</v>
       </c>
-      <c r="L34" s="29">
+      <c r="L34" s="10">
         <f t="shared" si="10"/>
         <v>72.222222222222229</v>
       </c>
-      <c r="M34" s="29">
+      <c r="M34" s="10">
         <f t="shared" si="15"/>
         <v>27.777777777777771</v>
       </c>
-      <c r="N34" s="31">
+      <c r="N34" s="23">
         <f t="shared" si="16"/>
         <v>26843.814285714281</v>
       </c>
       <c r="O34" s="2"/>
-      <c r="P34" s="6"/>
-    </row>
-    <row r="35" spans="1:16" ht="24" customHeight="1">
-      <c r="A35" s="9">
-        <v>35338</v>
-      </c>
-      <c r="B35" s="22">
+      <c r="P34" s="5"/>
+    </row>
+    <row r="35" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="8">
+        <v>41182</v>
+      </c>
+      <c r="B35" s="7">
         <v>5</v>
       </c>
-      <c r="C35" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D35" s="14">
+      <c r="C35" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35" s="13">
         <v>27</v>
       </c>
-      <c r="E35" s="16">
+      <c r="E35" s="15">
         <v>3</v>
       </c>
-      <c r="F35" s="18">
+      <c r="F35" s="17">
         <v>17</v>
       </c>
-      <c r="G35" s="22">
+      <c r="G35" s="7">
         <v>6</v>
       </c>
-      <c r="H35" s="15">
+      <c r="H35" s="14">
         <f t="shared" si="5"/>
         <v>32.400000000000006</v>
       </c>
-      <c r="I35" s="17">
+      <c r="I35" s="16">
         <f t="shared" si="6"/>
         <v>19.636363636363637</v>
       </c>
-      <c r="J35" s="19">
+      <c r="J35" s="18">
         <f t="shared" si="6"/>
         <v>111.27272727272727</v>
       </c>
-      <c r="K35" s="28">
+      <c r="K35" s="9">
         <f t="shared" si="9"/>
         <v>163.30909090909091</v>
       </c>
-      <c r="L35" s="29">
+      <c r="L35" s="10">
         <f t="shared" si="10"/>
         <v>85</v>
       </c>
-      <c r="M35" s="29">
+      <c r="M35" s="10">
         <f t="shared" si="15"/>
         <v>15</v>
       </c>
-      <c r="N35" s="31">
+      <c r="N35" s="23">
         <f t="shared" si="16"/>
         <v>27007.123376623371</v>
       </c>
       <c r="O35" s="2"/>
-      <c r="P35" s="6"/>
-    </row>
-    <row r="36" spans="1:16" ht="24" customHeight="1">
-      <c r="A36" s="9">
-        <v>35339</v>
-      </c>
-      <c r="B36" s="22">
+      <c r="P35" s="5"/>
+    </row>
+    <row r="36" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="8">
+        <v>41183</v>
+      </c>
+      <c r="B36" s="7">
         <v>4</v>
       </c>
-      <c r="C36" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D36" s="14">
+      <c r="C36" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36" s="13">
         <v>3</v>
       </c>
-      <c r="E36" s="16">
+      <c r="E36" s="15">
         <v>15</v>
       </c>
-      <c r="F36" s="18">
+      <c r="F36" s="17">
         <v>35</v>
       </c>
-      <c r="G36" s="22">
+      <c r="G36" s="7">
         <v>6</v>
       </c>
-      <c r="H36" s="15">
+      <c r="H36" s="14">
         <f t="shared" si="5"/>
         <v>4.5</v>
       </c>
-      <c r="I36" s="17">
+      <c r="I36" s="16">
         <f t="shared" si="6"/>
         <v>98.181818181818173</v>
       </c>
-      <c r="J36" s="19">
+      <c r="J36" s="18">
         <f t="shared" si="6"/>
         <v>229.09090909090909</v>
       </c>
-      <c r="K36" s="28">
+      <c r="K36" s="9">
         <f t="shared" si="9"/>
         <v>331.77272727272725</v>
       </c>
-      <c r="L36" s="29">
+      <c r="L36" s="10">
         <f t="shared" si="10"/>
         <v>70</v>
       </c>
-      <c r="M36" s="29">
+      <c r="M36" s="10">
         <f t="shared" si="15"/>
         <v>30</v>
       </c>
-      <c r="N36" s="31">
+      <c r="N36" s="23">
         <f t="shared" si="16"/>
         <v>27338.896103896099</v>
       </c>
       <c r="O36" s="2"/>
-      <c r="P36" s="6"/>
-    </row>
-    <row r="37" spans="1:16" ht="24" customHeight="1">
-      <c r="A37" s="9">
-        <v>35340</v>
-      </c>
-      <c r="B37" s="22">
+      <c r="P36" s="5"/>
+    </row>
+    <row r="37" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="8">
+        <v>41184</v>
+      </c>
+      <c r="B37" s="7">
         <v>5</v>
       </c>
-      <c r="C37" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D37" s="14">
+      <c r="C37" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37" s="13">
         <v>22</v>
       </c>
-      <c r="E37" s="16">
+      <c r="E37" s="15">
         <v>7</v>
       </c>
-      <c r="F37" s="18">
+      <c r="F37" s="17">
         <v>15</v>
       </c>
-      <c r="G37" s="22">
+      <c r="G37" s="7">
         <v>8</v>
       </c>
-      <c r="H37" s="15">
+      <c r="H37" s="14">
         <f t="shared" si="5"/>
         <v>35.200000000000003</v>
       </c>
-      <c r="I37" s="17">
+      <c r="I37" s="16">
         <f t="shared" si="6"/>
         <v>45.818181818181813</v>
       </c>
-      <c r="J37" s="19">
+      <c r="J37" s="18">
         <f t="shared" si="6"/>
         <v>98.181818181818173</v>
       </c>
-      <c r="K37" s="28">
+      <c r="K37" s="9">
         <f t="shared" si="9"/>
         <v>179.2</v>
       </c>
-      <c r="L37" s="29">
+      <c r="L37" s="10">
         <f t="shared" si="10"/>
         <v>68.181818181818173</v>
       </c>
-      <c r="M37" s="29">
+      <c r="M37" s="10">
         <f t="shared" si="15"/>
         <v>31.818181818181827</v>
       </c>
-      <c r="N37" s="31">
+      <c r="N37" s="23">
         <f t="shared" si="16"/>
         <v>27518.0961038961</v>
       </c>
-      <c r="O37" s="5"/>
-      <c r="P37" s="6"/>
-    </row>
-    <row r="38" spans="1:16" ht="18.75">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
-      <c r="I38" s="10">
+      <c r="O37" s="4"/>
+      <c r="P37" s="5"/>
+    </row>
+    <row r="38" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="9">
         <f>SUM(I6:I37)</f>
         <v>5465.4545454545441</v>
       </c>
-      <c r="J38" s="10">
+      <c r="J38" s="9">
         <f>SUM(J6:J37)</f>
         <v>16671.272727272728</v>
       </c>
-      <c r="K38" s="12"/>
-      <c r="L38" s="11">
+      <c r="K38" s="11"/>
+      <c r="L38" s="10">
         <f>SUM(J38)/(I38+J38)*100</f>
         <v>75.310467179183917</v>
       </c>
-      <c r="M38" s="29">
+      <c r="M38" s="10">
         <f t="shared" ref="M38" si="17">SUM(100-L38)</f>
         <v>24.689532820816083</v>
       </c>
-      <c r="N38" s="12"/>
+      <c r="N38" s="11"/>
       <c r="O38" s="1" t="s">
         <v>1</v>
       </c>
@@ -3315,24 +3322,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>